<commit_message>
excel and extent reports
</commit_message>
<xml_diff>
--- a/exceldata.xlsx
+++ b/exceldata.xlsx
@@ -380,13 +380,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>